<commit_message>
refactor:extract CaseFormat.py and Reasoning.py for common use
</commit_message>
<xml_diff>
--- a/DSMCaseReasoning/src/cases.xlsx
+++ b/DSMCaseReasoning/src/cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA32F411-5814-4960-8C22-B1DC659A7102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF33AB4-69B3-44D8-B1F9-9E5364A212E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2528" yWindow="1500" windowWidth="16199" windowHeight="9308" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="10" r:id="rId1"/>
-    <sheet name="Envs" sheetId="11" r:id="rId2"/>
+    <sheet name="formalization" sheetId="12" r:id="rId2"/>
+    <sheet name="Envs" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cases!$E$1:$E$190</definedName>
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="262">
   <si>
     <t>ID</t>
   </si>
@@ -1112,6 +1113,34 @@
   </si>
   <si>
     <t>Slope length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>discrete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>factors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>elevationD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1119,8 +1148,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1292,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1334,6 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1616,24 +1647,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4B5E7B-DB16-460C-8634-EAB54F114957}">
   <dimension ref="A1:J190"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="F195" sqref="F195"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.796875" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" customWidth="1"/>
+    <col min="10" max="10" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1665,7 +1696,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1697,7 +1728,7 @@
         <v>3313</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1729,7 +1760,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1761,7 +1792,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1793,7 +1824,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1825,7 +1856,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1857,7 +1888,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>16</v>
       </c>
@@ -1889,7 +1920,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1921,7 +1952,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>23</v>
       </c>
@@ -1953,7 +1984,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>24</v>
       </c>
@@ -1985,7 +2016,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>25</v>
       </c>
@@ -2017,7 +2048,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>26</v>
       </c>
@@ -2049,7 +2080,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>27</v>
       </c>
@@ -2081,7 +2112,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>30</v>
       </c>
@@ -2113,7 +2144,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>31</v>
       </c>
@@ -2145,7 +2176,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>32</v>
       </c>
@@ -2177,7 +2208,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>33</v>
       </c>
@@ -2209,7 +2240,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>34</v>
       </c>
@@ -2241,7 +2272,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>35</v>
       </c>
@@ -2273,7 +2304,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>38</v>
       </c>
@@ -2305,7 +2336,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>39</v>
       </c>
@@ -2337,7 +2368,7 @@
         <v>4316</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>41</v>
       </c>
@@ -2369,7 +2400,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>42</v>
       </c>
@@ -2401,7 +2432,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>43</v>
       </c>
@@ -2433,7 +2464,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>44</v>
       </c>
@@ -2465,7 +2496,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>45</v>
       </c>
@@ -2497,7 +2528,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>46</v>
       </c>
@@ -2529,7 +2560,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>47</v>
       </c>
@@ -2561,7 +2592,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>51</v>
       </c>
@@ -2593,7 +2624,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>52</v>
       </c>
@@ -2625,7 +2656,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>53</v>
       </c>
@@ -2657,7 +2688,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>54</v>
       </c>
@@ -2689,7 +2720,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>55</v>
       </c>
@@ -2721,7 +2752,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>56</v>
       </c>
@@ -2753,7 +2784,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>57</v>
       </c>
@@ -2785,7 +2816,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>58</v>
       </c>
@@ -2817,7 +2848,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>59</v>
       </c>
@@ -2849,7 +2880,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>60</v>
       </c>
@@ -2881,7 +2912,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>62</v>
       </c>
@@ -2913,7 +2944,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>63</v>
       </c>
@@ -2945,7 +2976,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>64</v>
       </c>
@@ -2977,7 +3008,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>65</v>
       </c>
@@ -3009,7 +3040,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>66</v>
       </c>
@@ -3041,7 +3072,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>67</v>
       </c>
@@ -3073,7 +3104,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>68</v>
       </c>
@@ -3105,7 +3136,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>69</v>
       </c>
@@ -3137,7 +3168,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>71</v>
       </c>
@@ -3169,7 +3200,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>72</v>
       </c>
@@ -3201,7 +3232,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>73</v>
       </c>
@@ -3233,7 +3264,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>74</v>
       </c>
@@ -3265,7 +3296,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>75</v>
       </c>
@@ -3297,7 +3328,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>76</v>
       </c>
@@ -3329,7 +3360,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>78</v>
       </c>
@@ -3361,7 +3392,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>79</v>
       </c>
@@ -3393,7 +3424,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>80</v>
       </c>
@@ -3425,7 +3456,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>81</v>
       </c>
@@ -3457,7 +3488,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>82</v>
       </c>
@@ -3489,7 +3520,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>83</v>
       </c>
@@ -3521,7 +3552,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>84</v>
       </c>
@@ -3553,7 +3584,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>85</v>
       </c>
@@ -3585,7 +3616,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>86</v>
       </c>
@@ -3617,7 +3648,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>87</v>
       </c>
@@ -3649,7 +3680,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>88</v>
       </c>
@@ -3681,7 +3712,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>89</v>
       </c>
@@ -3713,7 +3744,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>103</v>
       </c>
@@ -3745,7 +3776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>104</v>
       </c>
@@ -3777,7 +3808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>105</v>
       </c>
@@ -3809,7 +3840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>106</v>
       </c>
@@ -3841,7 +3872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>113</v>
       </c>
@@ -3873,7 +3904,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>114</v>
       </c>
@@ -3905,7 +3936,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>115</v>
       </c>
@@ -3937,7 +3968,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>116</v>
       </c>
@@ -3969,7 +4000,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>117</v>
       </c>
@@ -4001,7 +4032,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>118</v>
       </c>
@@ -4033,7 +4064,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>119</v>
       </c>
@@ -4065,7 +4096,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>120</v>
       </c>
@@ -4097,7 +4128,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>121</v>
       </c>
@@ -4129,7 +4160,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>122</v>
       </c>
@@ -4161,7 +4192,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>123</v>
       </c>
@@ -4193,7 +4224,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>124</v>
       </c>
@@ -4225,7 +4256,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>125</v>
       </c>
@@ -4257,7 +4288,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>127</v>
       </c>
@@ -4289,7 +4320,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>128</v>
       </c>
@@ -4321,7 +4352,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>129</v>
       </c>
@@ -4353,7 +4384,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>130</v>
       </c>
@@ -4385,7 +4416,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>131</v>
       </c>
@@ -4417,7 +4448,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>132</v>
       </c>
@@ -4449,7 +4480,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>133</v>
       </c>
@@ -4481,7 +4512,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>134</v>
       </c>
@@ -4513,7 +4544,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>135</v>
       </c>
@@ -4545,7 +4576,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>136</v>
       </c>
@@ -4577,7 +4608,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>138</v>
       </c>
@@ -4609,7 +4640,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>139</v>
       </c>
@@ -4641,7 +4672,7 @@
         <v>4718</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>141</v>
       </c>
@@ -4673,7 +4704,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>143</v>
       </c>
@@ -4705,7 +4736,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>144</v>
       </c>
@@ -4737,7 +4768,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>145</v>
       </c>
@@ -4769,7 +4800,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>147</v>
       </c>
@@ -4801,7 +4832,7 @@
         <v>658.7</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>149</v>
       </c>
@@ -4833,7 +4864,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>150</v>
       </c>
@@ -4865,7 +4896,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>151</v>
       </c>
@@ -4897,7 +4928,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>152</v>
       </c>
@@ -4929,7 +4960,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>153</v>
       </c>
@@ -4961,7 +4992,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>154</v>
       </c>
@@ -4993,7 +5024,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>155</v>
       </c>
@@ -5025,7 +5056,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>156</v>
       </c>
@@ -5057,7 +5088,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>157</v>
       </c>
@@ -5089,7 +5120,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>158</v>
       </c>
@@ -5121,7 +5152,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>159</v>
       </c>
@@ -5153,7 +5184,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>160</v>
       </c>
@@ -5185,7 +5216,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>166</v>
       </c>
@@ -5217,7 +5248,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>167</v>
       </c>
@@ -5249,7 +5280,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>168</v>
       </c>
@@ -5281,7 +5312,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>169</v>
       </c>
@@ -5313,7 +5344,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>170</v>
       </c>
@@ -5345,7 +5376,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>174</v>
       </c>
@@ -5377,7 +5408,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>175</v>
       </c>
@@ -5409,7 +5440,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>176</v>
       </c>
@@ -5441,7 +5472,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>177</v>
       </c>
@@ -5473,7 +5504,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>178</v>
       </c>
@@ -5505,7 +5536,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>179</v>
       </c>
@@ -5537,7 +5568,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>180</v>
       </c>
@@ -5569,7 +5600,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>181</v>
       </c>
@@ -5601,7 +5632,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>182</v>
       </c>
@@ -5633,7 +5664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>183</v>
       </c>
@@ -5665,7 +5696,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>184</v>
       </c>
@@ -5697,7 +5728,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>185</v>
       </c>
@@ -5729,7 +5760,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>186</v>
       </c>
@@ -5761,7 +5792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>187</v>
       </c>
@@ -5793,7 +5824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>188</v>
       </c>
@@ -5825,7 +5856,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>189</v>
       </c>
@@ -5857,7 +5888,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>190</v>
       </c>
@@ -5889,7 +5920,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>191</v>
       </c>
@@ -5921,7 +5952,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>197</v>
       </c>
@@ -5953,7 +5984,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>198</v>
       </c>
@@ -5985,7 +6016,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>199</v>
       </c>
@@ -6017,7 +6048,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>200</v>
       </c>
@@ -6049,7 +6080,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>201</v>
       </c>
@@ -6081,7 +6112,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>202</v>
       </c>
@@ -6113,7 +6144,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>203</v>
       </c>
@@ -6145,7 +6176,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>204</v>
       </c>
@@ -6177,7 +6208,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>205</v>
       </c>
@@ -6209,7 +6240,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>206</v>
       </c>
@@ -6241,7 +6272,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>207</v>
       </c>
@@ -6273,7 +6304,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>208</v>
       </c>
@@ -6305,7 +6336,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A147">
         <v>209</v>
       </c>
@@ -6337,7 +6368,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A148">
         <v>210</v>
       </c>
@@ -6369,7 +6400,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>211</v>
       </c>
@@ -6401,7 +6432,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A150">
         <v>212</v>
       </c>
@@ -6433,7 +6464,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A151">
         <v>213</v>
       </c>
@@ -6465,7 +6496,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A152">
         <v>214</v>
       </c>
@@ -6497,7 +6528,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A153">
         <v>215</v>
       </c>
@@ -6529,7 +6560,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A154">
         <v>216</v>
       </c>
@@ -6561,7 +6592,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A155">
         <v>217</v>
       </c>
@@ -6593,7 +6624,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A156">
         <v>218</v>
       </c>
@@ -6625,7 +6656,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A157">
         <v>219</v>
       </c>
@@ -6657,7 +6688,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A158">
         <v>220</v>
       </c>
@@ -6689,7 +6720,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A159">
         <v>221</v>
       </c>
@@ -6721,7 +6752,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A160">
         <v>222</v>
       </c>
@@ -6753,7 +6784,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A161">
         <v>223</v>
       </c>
@@ -6785,7 +6816,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A162">
         <v>224</v>
       </c>
@@ -6817,7 +6848,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A163">
         <v>225</v>
       </c>
@@ -6849,7 +6880,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A164">
         <v>226</v>
       </c>
@@ -6881,7 +6912,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A165">
         <v>227</v>
       </c>
@@ -6913,7 +6944,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A166">
         <v>228</v>
       </c>
@@ -6945,7 +6976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A167">
         <v>229</v>
       </c>
@@ -6977,7 +7008,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A168">
         <v>230</v>
       </c>
@@ -7009,7 +7040,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A169">
         <v>231</v>
       </c>
@@ -7041,7 +7072,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A170">
         <v>232</v>
       </c>
@@ -7073,7 +7104,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A171">
         <v>233</v>
       </c>
@@ -7105,7 +7136,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A172">
         <v>234</v>
       </c>
@@ -7137,7 +7168,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A173">
         <v>235</v>
       </c>
@@ -7169,7 +7200,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A174">
         <v>236</v>
       </c>
@@ -7201,7 +7232,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A175">
         <v>237</v>
       </c>
@@ -7233,7 +7264,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A176">
         <v>238</v>
       </c>
@@ -7265,7 +7296,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A177">
         <v>239</v>
       </c>
@@ -7297,7 +7328,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A178">
         <v>240</v>
       </c>
@@ -7329,7 +7360,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A179">
         <v>248</v>
       </c>
@@ -7361,7 +7392,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A180">
         <v>249</v>
       </c>
@@ -7393,7 +7424,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A181">
         <v>250</v>
       </c>
@@ -7425,7 +7456,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A182">
         <v>251</v>
       </c>
@@ -7457,7 +7488,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A183">
         <v>252</v>
       </c>
@@ -7489,7 +7520,7 @@
         <v>87.316000000000003</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A184">
         <v>253</v>
       </c>
@@ -7521,7 +7552,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A185">
         <v>254</v>
       </c>
@@ -7553,7 +7584,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A186">
         <v>255</v>
       </c>
@@ -7585,7 +7616,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A187">
         <v>256</v>
       </c>
@@ -7617,7 +7648,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A188">
         <v>257</v>
       </c>
@@ -7649,7 +7680,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A189">
         <v>258</v>
       </c>
@@ -7681,7 +7712,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A190">
         <v>259</v>
       </c>
@@ -7724,40 +7755,148 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55686D-E9BA-4AA5-919E-3E3ED25FC328}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="8" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="23">
+        <v>200</v>
+      </c>
+      <c r="C3" s="23">
+        <v>200</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23">
+        <v>2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="G3" s="23">
+        <v>2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>20</v>
+      </c>
+      <c r="I3" s="23">
+        <v>8848</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B7A103-8910-40A2-A97F-D6DE2A9F3FC6}">
   <dimension ref="A1:X190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.1328125" customWidth="1"/>
+    <col min="4" max="4" width="27.19921875" customWidth="1"/>
+    <col min="5" max="5" width="32.86328125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.86328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.46484375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.46484375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7831,7 +7970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -7878,7 +8017,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>6</v>
       </c>
@@ -7907,7 +8046,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7918,7 +8057,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>11</v>
       </c>
@@ -7935,7 +8074,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>12</v>
       </c>
@@ -7946,7 +8085,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>15</v>
       </c>
@@ -7954,7 +8093,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>16</v>
       </c>
@@ -7962,7 +8101,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>20</v>
       </c>
@@ -7970,7 +8109,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>23</v>
       </c>
@@ -7978,7 +8117,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>24</v>
       </c>
@@ -7986,7 +8125,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>25</v>
       </c>
@@ -8000,7 +8139,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>26</v>
       </c>
@@ -8011,7 +8150,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>27</v>
       </c>
@@ -8019,7 +8158,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>30</v>
       </c>
@@ -8027,7 +8166,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>31</v>
       </c>
@@ -8038,7 +8177,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>32</v>
       </c>
@@ -8049,7 +8188,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>33</v>
       </c>
@@ -8060,7 +8199,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>34</v>
       </c>
@@ -8071,7 +8210,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>35</v>
       </c>
@@ -8079,7 +8218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>38</v>
       </c>
@@ -8123,7 +8262,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>39</v>
       </c>
@@ -8152,7 +8291,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>41</v>
       </c>
@@ -8184,7 +8323,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>42</v>
       </c>
@@ -8216,7 +8355,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>43</v>
       </c>
@@ -8254,7 +8393,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>44</v>
       </c>
@@ -8289,7 +8428,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>45</v>
       </c>
@@ -8324,7 +8463,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>46</v>
       </c>
@@ -8338,7 +8477,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>47</v>
       </c>
@@ -8363,7 +8502,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>51</v>
       </c>
@@ -8377,7 +8516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>52</v>
       </c>
@@ -8394,7 +8533,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>53</v>
       </c>
@@ -8420,7 +8559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>54</v>
       </c>
@@ -8440,7 +8579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>55</v>
       </c>
@@ -8469,7 +8608,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>56</v>
       </c>
@@ -8498,7 +8637,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>57</v>
       </c>
@@ -8526,7 +8665,7 @@
       <c r="M36" s="20"/>
       <c r="N36" s="20"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>58</v>
       </c>
@@ -8555,7 +8694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>59</v>
       </c>
@@ -8587,7 +8726,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>60</v>
       </c>
@@ -8616,7 +8755,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>62</v>
       </c>
@@ -8654,7 +8793,7 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>63</v>
       </c>
@@ -8680,7 +8819,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>64</v>
       </c>
@@ -8707,7 +8846,7 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>65</v>
       </c>
@@ -8757,7 +8896,7 @@
       <c r="W43" s="14"/>
       <c r="X43" s="14"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>66</v>
       </c>
@@ -8807,7 +8946,7 @@
       <c r="W44" s="14"/>
       <c r="X44" s="14"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>67</v>
       </c>
@@ -8857,7 +8996,7 @@
       <c r="W45" s="14"/>
       <c r="X45" s="14"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>68</v>
       </c>
@@ -8907,7 +9046,7 @@
       <c r="W46" s="14"/>
       <c r="X46" s="14"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>69</v>
       </c>
@@ -8957,7 +9096,7 @@
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>71</v>
       </c>
@@ -8983,7 +9122,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>72</v>
       </c>
@@ -9030,7 +9169,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>73</v>
       </c>
@@ -9077,7 +9216,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>74</v>
       </c>
@@ -9124,7 +9263,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>75</v>
       </c>
@@ -9171,7 +9310,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>76</v>
       </c>
@@ -9218,7 +9357,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>78</v>
       </c>
@@ -9274,7 +9413,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>79</v>
       </c>
@@ -9330,7 +9469,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>80</v>
       </c>
@@ -9386,7 +9525,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>81</v>
       </c>
@@ -9444,7 +9583,7 @@
       <c r="W57" s="9"/>
       <c r="X57" s="9"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>82</v>
       </c>
@@ -9508,7 +9647,7 @@
       <c r="W58" s="8"/>
       <c r="X58" s="9"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>83</v>
       </c>
@@ -9572,7 +9711,7 @@
       <c r="W59" s="9"/>
       <c r="X59" s="8"/>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>84</v>
       </c>
@@ -9626,7 +9765,7 @@
       <c r="W60" s="9"/>
       <c r="X60" s="9"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>85</v>
       </c>
@@ -9680,7 +9819,7 @@
       <c r="U61" s="9"/>
       <c r="V61" s="9"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>86</v>
       </c>
@@ -9747,7 +9886,7 @@
       <c r="W62" s="8"/>
       <c r="X62" s="9"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>87</v>
       </c>
@@ -9784,7 +9923,7 @@
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>88</v>
       </c>
@@ -9829,7 +9968,7 @@
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>89</v>
       </c>
@@ -9882,7 +10021,7 @@
       <c r="T65" s="9"/>
       <c r="U65" s="8"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>103</v>
       </c>
@@ -9917,7 +10056,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>104</v>
       </c>
@@ -9949,7 +10088,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>105</v>
       </c>
@@ -9987,7 +10126,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>106</v>
       </c>
@@ -10019,7 +10158,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>113</v>
       </c>
@@ -10057,7 +10196,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>114</v>
       </c>
@@ -10089,7 +10228,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>115</v>
       </c>
@@ -10124,7 +10263,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>116</v>
       </c>
@@ -10156,7 +10295,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>117</v>
       </c>
@@ -10167,7 +10306,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>118</v>
       </c>
@@ -10184,7 +10323,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>119</v>
       </c>
@@ -10198,7 +10337,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>120</v>
       </c>
@@ -10212,7 +10351,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>121</v>
       </c>
@@ -10232,7 +10371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>122</v>
       </c>
@@ -10252,7 +10391,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>123</v>
       </c>
@@ -10266,7 +10405,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>124</v>
       </c>
@@ -10280,7 +10419,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>125</v>
       </c>
@@ -10312,7 +10451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>127</v>
       </c>
@@ -10377,7 +10516,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>128</v>
       </c>
@@ -10442,7 +10581,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>129</v>
       </c>
@@ -10478,7 +10617,7 @@
       <c r="O85" s="9"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>130</v>
       </c>
@@ -10514,7 +10653,7 @@
       <c r="O86" s="9"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>131</v>
       </c>
@@ -10550,7 +10689,7 @@
       <c r="O87" s="9"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>132</v>
       </c>
@@ -10586,7 +10725,7 @@
       <c r="O88" s="9"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>133</v>
       </c>
@@ -10654,7 +10793,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>134</v>
       </c>
@@ -10723,7 +10862,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>135</v>
       </c>
@@ -10761,7 +10900,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>136</v>
       </c>
@@ -10799,7 +10938,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>138</v>
       </c>
@@ -10840,7 +10979,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="94" spans="1:24" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>139</v>
       </c>
@@ -10866,7 +11005,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>141</v>
       </c>
@@ -10892,7 +11031,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>143</v>
       </c>
@@ -10921,7 +11060,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>144</v>
       </c>
@@ -10950,7 +11089,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>145</v>
       </c>
@@ -10970,7 +11109,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>147</v>
       </c>
@@ -10995,7 +11134,7 @@
       <c r="N99" s="9"/>
       <c r="O99" s="8"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>149</v>
       </c>
@@ -11019,7 +11158,7 @@
       </c>
       <c r="H100" s="8"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>150</v>
       </c>
@@ -11045,7 +11184,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>151</v>
       </c>
@@ -11083,7 +11222,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>152</v>
       </c>
@@ -11112,7 +11251,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>153</v>
       </c>
@@ -11144,7 +11283,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>154</v>
       </c>
@@ -11176,7 +11315,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>155</v>
       </c>
@@ -11193,7 +11332,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>156</v>
       </c>
@@ -11210,7 +11349,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>157</v>
       </c>
@@ -11224,7 +11363,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>158</v>
       </c>
@@ -11235,7 +11374,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>159</v>
       </c>
@@ -11249,7 +11388,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>160</v>
       </c>
@@ -11269,7 +11408,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>166</v>
       </c>
@@ -11296,7 +11435,7 @@
       </c>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>167</v>
       </c>
@@ -11323,7 +11462,7 @@
       </c>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>168</v>
       </c>
@@ -11350,7 +11489,7 @@
       </c>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>169</v>
       </c>
@@ -11377,7 +11516,7 @@
       </c>
       <c r="I115" s="9"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>170</v>
       </c>
@@ -11404,7 +11543,7 @@
       </c>
       <c r="I116" s="9"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>174</v>
       </c>
@@ -11463,7 +11602,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>175</v>
       </c>
@@ -11519,7 +11658,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>176</v>
       </c>
@@ -11575,7 +11714,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>177</v>
       </c>
@@ -11622,7 +11761,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>178</v>
       </c>
@@ -11663,7 +11802,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>179</v>
       </c>
@@ -11717,7 +11856,7 @@
       </c>
       <c r="R122" s="15"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>180</v>
       </c>
@@ -11771,7 +11910,7 @@
       </c>
       <c r="R123" s="15"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>181</v>
       </c>
@@ -11825,7 +11964,7 @@
       </c>
       <c r="R124" s="15"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>182</v>
       </c>
@@ -11879,7 +12018,7 @@
       </c>
       <c r="R125" s="15"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>183</v>
       </c>
@@ -11933,7 +12072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>184</v>
       </c>
@@ -11986,7 +12125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>185</v>
       </c>
@@ -12036,7 +12175,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>186</v>
       </c>
@@ -12086,7 +12225,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>187</v>
       </c>
@@ -12094,7 +12233,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>188</v>
       </c>
@@ -12102,7 +12241,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>189</v>
       </c>
@@ -12116,7 +12255,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>190</v>
       </c>
@@ -12145,7 +12284,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>191</v>
       </c>
@@ -12165,7 +12304,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>197</v>
       </c>
@@ -12218,7 +12357,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>198</v>
       </c>
@@ -12271,7 +12410,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>199</v>
       </c>
@@ -12324,7 +12463,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>200</v>
       </c>
@@ -12377,7 +12516,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>201</v>
       </c>
@@ -12395,7 +12534,7 @@
       <c r="G139" s="9"/>
       <c r="H139" s="9"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>202</v>
       </c>
@@ -12415,7 +12554,7 @@
       <c r="G140" s="9"/>
       <c r="H140" s="9"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>203</v>
       </c>
@@ -12429,7 +12568,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>204</v>
       </c>
@@ -12443,7 +12582,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>205</v>
       </c>
@@ -12484,7 +12623,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>206</v>
       </c>
@@ -12525,7 +12664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>207</v>
       </c>
@@ -12542,7 +12681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>208</v>
       </c>
@@ -12586,7 +12725,7 @@
       <c r="P146" s="9"/>
       <c r="Q146" s="9"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A147">
         <v>209</v>
       </c>
@@ -12634,7 +12773,7 @@
       </c>
       <c r="Q147" s="7"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A148">
         <v>210</v>
       </c>
@@ -12681,7 +12820,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>211</v>
       </c>
@@ -12728,7 +12867,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A150">
         <v>212</v>
       </c>
@@ -12757,7 +12896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A151">
         <v>213</v>
       </c>
@@ -12786,7 +12925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A152">
         <v>214</v>
       </c>
@@ -12815,7 +12954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A153">
         <v>215</v>
       </c>
@@ -12844,7 +12983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A154">
         <v>216</v>
       </c>
@@ -12879,7 +13018,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A155">
         <v>217</v>
       </c>
@@ -12911,7 +13050,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A156">
         <v>218</v>
       </c>
@@ -12943,7 +13082,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A157">
         <v>219</v>
       </c>
@@ -12981,7 +13120,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A158">
         <v>220</v>
       </c>
@@ -13013,7 +13152,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A159">
         <v>221</v>
       </c>
@@ -13033,7 +13172,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A160">
         <v>222</v>
       </c>
@@ -13059,7 +13198,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A161">
         <v>223</v>
       </c>
@@ -13112,7 +13251,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A162">
         <v>224</v>
       </c>
@@ -13132,7 +13271,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A163">
         <v>225</v>
       </c>
@@ -13152,7 +13291,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A164">
         <v>226</v>
       </c>
@@ -13166,7 +13305,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A165">
         <v>227</v>
       </c>
@@ -13186,7 +13325,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A166">
         <v>228</v>
       </c>
@@ -13200,7 +13339,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A167">
         <v>229</v>
       </c>
@@ -13211,7 +13350,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A168">
         <v>230</v>
       </c>
@@ -13225,7 +13364,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A169">
         <v>231</v>
       </c>
@@ -13233,7 +13372,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A170">
         <v>232</v>
       </c>
@@ -13271,7 +13410,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A171">
         <v>233</v>
       </c>
@@ -13300,7 +13439,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A172">
         <v>234</v>
       </c>
@@ -13332,7 +13471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A173">
         <v>235</v>
       </c>
@@ -13364,7 +13503,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A174">
         <v>236</v>
       </c>
@@ -13390,7 +13529,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A175">
         <v>237</v>
       </c>
@@ -13431,7 +13570,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A176">
         <v>238</v>
       </c>
@@ -13448,7 +13587,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A177">
         <v>239</v>
       </c>
@@ -13477,7 +13616,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A178">
         <v>240</v>
       </c>
@@ -13512,7 +13651,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A179">
         <v>248</v>
       </c>
@@ -13538,7 +13677,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A180">
         <v>249</v>
       </c>
@@ -13564,7 +13703,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A181">
         <v>250</v>
       </c>
@@ -13590,7 +13729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A182">
         <v>251</v>
       </c>
@@ -13607,7 +13746,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A183">
         <v>252</v>
       </c>
@@ -13630,7 +13769,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A184">
         <v>253</v>
       </c>
@@ -13650,7 +13789,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A185">
         <v>254</v>
       </c>
@@ -13682,7 +13821,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A186">
         <v>255</v>
       </c>
@@ -13702,7 +13841,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A187">
         <v>256</v>
       </c>
@@ -13740,7 +13879,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A188">
         <v>257</v>
       </c>
@@ -13763,7 +13902,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A189">
         <v>258</v>
       </c>
@@ -13792,7 +13931,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A190">
         <v>259</v>
       </c>

</xml_diff>

<commit_message>
fix(case_csv): Replace dem with filled_dem
</commit_message>
<xml_diff>
--- a/DSMCaseReasoning/src/cases.xlsx
+++ b/DSMCaseReasoning/src/cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26708"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4565347-D89A-4E94-B132-491072D27005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607257D3-B11B-487D-8FB3-706F85AAE912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="6045" windowWidth="22515" windowHeight="12270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="10" r:id="rId1"/>
@@ -1060,10 +1060,10 @@
     <t>the ratio of annual precipitation and annual potential evapotranstream_power_indexration</t>
   </si>
   <si>
-    <t>dem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dem </t>
+    <t>filled_dem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filled_dem </t>
   </si>
 </sst>
 </file>
@@ -1566,20 +1566,20 @@
       <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.73046875" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.265625" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
-    <col min="10" max="10" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.75" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="17.125" customWidth="1"/>
+    <col min="9" max="9" width="10.75" customWidth="1"/>
+    <col min="10" max="10" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>3313</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>23</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>24</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>26</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>27</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>35</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>38</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>39</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>4316</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>41</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>42</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>43</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>44</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>45</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>46</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>47</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>51</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>52</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>53</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>54</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>55</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>56</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>57</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>59</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>60</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>62</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>63</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>64</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>65</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>66</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>67</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>68</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>69</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>71</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>72</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>73</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>74</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>75</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>76</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>78</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>79</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>80</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>81</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>82</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>83</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>84</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>85</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>86</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>87</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>88</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>89</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>103</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>104</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>105</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>106</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>113</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>114</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>115</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>116</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>117</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>118</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>119</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>120</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>121</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>122</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>123</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>124</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>125</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>127</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>128</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>129</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>130</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>131</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>132</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>133</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>134</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>135</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>136</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>138</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>139</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>4718</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>141</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>143</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>144</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>145</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>147</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>658.7</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>149</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>150</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>151</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>152</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>153</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>154</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>155</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>156</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>157</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>158</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>159</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>160</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>166</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>167</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>168</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>169</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>170</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>174</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>175</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>176</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>177</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>178</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>179</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>180</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>181</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>182</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>183</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>184</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>185</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>186</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>187</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>188</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>189</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>190</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>191</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>197</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>198</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>199</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>200</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>201</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>202</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>203</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>204</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>205</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>206</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>207</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>208</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>209</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>210</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>211</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>212</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>213</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>214</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>215</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>216</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>217</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>218</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>219</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>220</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>221</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>222</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>223</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>224</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>225</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>226</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>227</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>228</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>229</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>230</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>231</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>232</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>233</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>234</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>235</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>236</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>237</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>238</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>239</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>240</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>248</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>249</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>250</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>251</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>252</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>87.316000000000003</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>253</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>254</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>255</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>256</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>257</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>258</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>259</v>
       </c>
@@ -7677,13 +7677,13 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="8" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>228</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>226</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>227</v>
       </c>
@@ -7781,37 +7781,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B7A103-8910-40A2-A97F-D6DE2A9F3FC6}">
   <dimension ref="A1:X190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H185" sqref="H185"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.59765625" customWidth="1"/>
-    <col min="3" max="3" width="32.1328125" customWidth="1"/>
-    <col min="4" max="4" width="27.265625" customWidth="1"/>
-    <col min="5" max="5" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="3" max="3" width="32.125" customWidth="1"/>
+    <col min="4" max="4" width="27.25" customWidth="1"/>
+    <col min="5" max="5" width="32.875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="40.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.86328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="28.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>23</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>24</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>26</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>27</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>35</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>38</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>39</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>41</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>42</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>43</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>44</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>45</v>
       </c>
@@ -8378,7 +8378,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>46</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>47</v>
       </c>
@@ -8417,7 +8417,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>51</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>52</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>53</v>
       </c>
@@ -8474,7 +8474,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>54</v>
       </c>
@@ -8494,7 +8494,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>55</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>56</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>57</v>
       </c>
@@ -8580,7 +8580,7 @@
       <c r="M36" s="20"/>
       <c r="N36" s="20"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>59</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>60</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>62</v>
       </c>
@@ -8708,7 +8708,7 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>63</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>64</v>
       </c>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>65</v>
       </c>
@@ -8811,7 +8811,7 @@
       <c r="W43" s="14"/>
       <c r="X43" s="14"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>66</v>
       </c>
@@ -8861,7 +8861,7 @@
       <c r="W44" s="14"/>
       <c r="X44" s="14"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>67</v>
       </c>
@@ -8911,7 +8911,7 @@
       <c r="W45" s="14"/>
       <c r="X45" s="14"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>68</v>
       </c>
@@ -8961,7 +8961,7 @@
       <c r="W46" s="14"/>
       <c r="X46" s="14"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>69</v>
       </c>
@@ -9011,7 +9011,7 @@
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>71</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>72</v>
       </c>
@@ -9084,7 +9084,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>73</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>74</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>75</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>76</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>78</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>79</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>80</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>81</v>
       </c>
@@ -9498,7 +9498,7 @@
       <c r="W57" s="9"/>
       <c r="X57" s="9"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>82</v>
       </c>
@@ -9562,7 +9562,7 @@
       <c r="W58" s="8"/>
       <c r="X58" s="9"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>83</v>
       </c>
@@ -9626,7 +9626,7 @@
       <c r="W59" s="9"/>
       <c r="X59" s="8"/>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>84</v>
       </c>
@@ -9680,7 +9680,7 @@
       <c r="W60" s="9"/>
       <c r="X60" s="9"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>85</v>
       </c>
@@ -9734,7 +9734,7 @@
       <c r="U61" s="9"/>
       <c r="V61" s="9"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>86</v>
       </c>
@@ -9801,7 +9801,7 @@
       <c r="W62" s="8"/>
       <c r="X62" s="9"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>87</v>
       </c>
@@ -9838,7 +9838,7 @@
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>88</v>
       </c>
@@ -9883,7 +9883,7 @@
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>89</v>
       </c>
@@ -9936,7 +9936,7 @@
       <c r="T65" s="9"/>
       <c r="U65" s="8"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>103</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>104</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>105</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>106</v>
       </c>
@@ -10073,7 +10073,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>113</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>114</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>115</v>
       </c>
@@ -10178,7 +10178,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>116</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>117</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>118</v>
       </c>
@@ -10238,7 +10238,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>119</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>120</v>
       </c>
@@ -10266,7 +10266,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>121</v>
       </c>
@@ -10286,7 +10286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>122</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>123</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>124</v>
       </c>
@@ -10334,7 +10334,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>125</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>127</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>128</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>129</v>
       </c>
@@ -10532,7 +10532,7 @@
       <c r="O85" s="9"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>130</v>
       </c>
@@ -10568,7 +10568,7 @@
       <c r="O86" s="9"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>131</v>
       </c>
@@ -10604,7 +10604,7 @@
       <c r="O87" s="9"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>132</v>
       </c>
@@ -10640,7 +10640,7 @@
       <c r="O88" s="9"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>133</v>
       </c>
@@ -10708,7 +10708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>134</v>
       </c>
@@ -10777,7 +10777,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>135</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>136</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>138</v>
       </c>
@@ -10894,7 +10894,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:24" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>139</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>141</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>143</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>144</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>145</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>147</v>
       </c>
@@ -11049,7 +11049,7 @@
       <c r="N99" s="9"/>
       <c r="O99" s="8"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>149</v>
       </c>
@@ -11073,7 +11073,7 @@
       </c>
       <c r="H100" s="8"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>150</v>
       </c>
@@ -11099,7 +11099,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>151</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>152</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>153</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>154</v>
       </c>
@@ -11230,7 +11230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>155</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>156</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>157</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>158</v>
       </c>
@@ -11289,7 +11289,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>159</v>
       </c>
@@ -11303,7 +11303,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>160</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>166</v>
       </c>
@@ -11350,7 +11350,7 @@
       </c>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>167</v>
       </c>
@@ -11377,7 +11377,7 @@
       </c>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>168</v>
       </c>
@@ -11404,7 +11404,7 @@
       </c>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>169</v>
       </c>
@@ -11431,7 +11431,7 @@
       </c>
       <c r="I115" s="9"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>170</v>
       </c>
@@ -11458,7 +11458,7 @@
       </c>
       <c r="I116" s="9"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>174</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>175</v>
       </c>
@@ -11573,7 +11573,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>176</v>
       </c>
@@ -11629,7 +11629,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>177</v>
       </c>
@@ -11676,7 +11676,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>178</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>179</v>
       </c>
@@ -11771,7 +11771,7 @@
       </c>
       <c r="R122" s="15"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>180</v>
       </c>
@@ -11825,7 +11825,7 @@
       </c>
       <c r="R123" s="15"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>181</v>
       </c>
@@ -11879,7 +11879,7 @@
       </c>
       <c r="R124" s="15"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>182</v>
       </c>
@@ -11933,7 +11933,7 @@
       </c>
       <c r="R125" s="15"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>183</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>184</v>
       </c>
@@ -12040,7 +12040,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>185</v>
       </c>
@@ -12090,7 +12090,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>186</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>187</v>
       </c>
@@ -12148,7 +12148,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>188</v>
       </c>
@@ -12156,7 +12156,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>189</v>
       </c>
@@ -12170,7 +12170,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>190</v>
       </c>
@@ -12199,7 +12199,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>191</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>197</v>
       </c>
@@ -12272,7 +12272,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>198</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>199</v>
       </c>
@@ -12378,7 +12378,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>200</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>201</v>
       </c>
@@ -12449,7 +12449,7 @@
       <c r="G139" s="9"/>
       <c r="H139" s="9"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>202</v>
       </c>
@@ -12469,7 +12469,7 @@
       <c r="G140" s="9"/>
       <c r="H140" s="9"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>203</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>204</v>
       </c>
@@ -12497,7 +12497,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>205</v>
       </c>
@@ -12538,7 +12538,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>206</v>
       </c>
@@ -12579,7 +12579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>207</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>208</v>
       </c>
@@ -12640,7 +12640,7 @@
       <c r="P146" s="9"/>
       <c r="Q146" s="9"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>209</v>
       </c>
@@ -12688,7 +12688,7 @@
       </c>
       <c r="Q147" s="7"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>210</v>
       </c>
@@ -12735,7 +12735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>211</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>212</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>213</v>
       </c>
@@ -12840,7 +12840,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>214</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>215</v>
       </c>
@@ -12898,7 +12898,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>216</v>
       </c>
@@ -12933,7 +12933,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>217</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>218</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>219</v>
       </c>
@@ -13035,7 +13035,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>220</v>
       </c>
@@ -13067,7 +13067,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>221</v>
       </c>
@@ -13087,7 +13087,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>222</v>
       </c>
@@ -13113,7 +13113,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>223</v>
       </c>
@@ -13166,7 +13166,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>224</v>
       </c>
@@ -13186,7 +13186,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>225</v>
       </c>
@@ -13206,7 +13206,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>226</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>227</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>228</v>
       </c>
@@ -13254,7 +13254,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>229</v>
       </c>
@@ -13265,7 +13265,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>230</v>
       </c>
@@ -13279,7 +13279,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>231</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>232</v>
       </c>
@@ -13325,7 +13325,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>233</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>234</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>235</v>
       </c>
@@ -13418,7 +13418,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>236</v>
       </c>
@@ -13444,7 +13444,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>237</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>238</v>
       </c>
@@ -13502,7 +13502,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>239</v>
       </c>
@@ -13531,7 +13531,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>240</v>
       </c>
@@ -13566,7 +13566,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>248</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>249</v>
       </c>
@@ -13618,7 +13618,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>250</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>251</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>252</v>
       </c>
@@ -13682,7 +13682,7 @@
       </c>
       <c r="G183" s="6"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>253</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>254</v>
       </c>
@@ -13731,7 +13731,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>255</v>
       </c>
@@ -13751,7 +13751,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>256</v>
       </c>
@@ -13789,7 +13789,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>257</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>258</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>259</v>
       </c>

</xml_diff>